<commit_message>
Fix handling of subpackages, that items don't appear twice.
</commit_message>
<xml_diff>
--- a/Examples/TraceScanner.xlsx
+++ b/Examples/TraceScanner.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="25875" windowHeight="11820"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="25875" windowHeight="11820" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="TraceScanner" sheetId="1" r:id="rId1"/>
+    <sheet name="WithPackages" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="113">
   <si>
     <t>Model</t>
   </si>
@@ -313,6 +312,48 @@
   </si>
   <si>
     <t>UML:Model &gt; UML:Package &gt; UML:Collaboration &gt; UML:ClassifierRole</t>
+  </si>
+  <si>
+    <t>Main Requirements</t>
+  </si>
+  <si>
+    <t>General Requirements</t>
+  </si>
+  <si>
+    <t>MX_EAID_74C4E2A8_AFF6_4d3c_B069_074FD2634DB0</t>
+  </si>
+  <si>
+    <t>EA Model</t>
+  </si>
+  <si>
+    <t>EAID_597BC40D_774D_48a1_ADDB_9D9B4CB3B729</t>
+  </si>
+  <si>
+    <t>package2</t>
+  </si>
+  <si>
+    <t>UML:Model &gt; UML:Package &gt; UML:Package</t>
+  </si>
+  <si>
+    <t>UML:Model &gt; UML:Package &gt; UML:Package &gt; UML:Collaboration &gt; UML:ClassifierRole</t>
+  </si>
+  <si>
+    <t>EAID_6863F3B8_847E_44fd_89A1_BB8DE33F0BFA</t>
+  </si>
+  <si>
+    <t>EAID_6A15D30D_ABCB_49d5_8DD5_2F5640E289FF</t>
+  </si>
+  <si>
+    <t>UML:Model &gt; UML:Package &gt; UML:Package &gt; UML:Package</t>
+  </si>
+  <si>
+    <t>EAPK_6A15D30D_ABCB_49d5_8DD5_2F5640E289FF</t>
+  </si>
+  <si>
+    <t>UML:Model &gt; UML:Package &gt; UML:Package &gt; UML:Package &gt; UML:Collaboration &gt; UML:ClassifierRole</t>
+  </si>
+  <si>
+    <t>EAPK_6863F3B8_847E_44fd_89A1_BB8DE33F0BFA</t>
   </si>
 </sst>
 </file>
@@ -346,12 +387,78 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -366,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -428,11 +535,70 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="6"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,17 +902,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="44.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.28515625" style="7" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="36" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32" style="1" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="3.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="6.85546875" style="7" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="33.28515625" style="1" hidden="1" customWidth="1"/>
@@ -756,57 +922,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D1" s="23" t="s">
+      <c r="A1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23" t="s">
+      <c r="E1" s="30"/>
+      <c r="F1" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="34" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>96</v>
@@ -880,7 +1049,7 @@
       <c r="G5" s="7">
         <v>2</v>
       </c>
-      <c r="J5" s="24" t="s">
+      <c r="J5" s="23" t="s">
         <v>41</v>
       </c>
     </row>
@@ -909,7 +1078,7 @@
       <c r="J6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="24" t="s">
+      <c r="K6" s="23" t="s">
         <v>53</v>
       </c>
     </row>
@@ -938,7 +1107,7 @@
       <c r="J7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="24" t="s">
+      <c r="K7" s="23" t="s">
         <v>59</v>
       </c>
     </row>
@@ -967,7 +1136,7 @@
       <c r="J8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K8" s="24" t="s">
+      <c r="K8" s="23" t="s">
         <v>59</v>
       </c>
     </row>
@@ -996,7 +1165,7 @@
       <c r="J9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="24" t="s">
+      <c r="K9" s="23" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1025,7 +1194,7 @@
       <c r="J10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K10" s="24" t="s">
+      <c r="K10" s="23" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1055,7 +1224,7 @@
       <c r="J11" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="K11" s="25" t="s">
+      <c r="K11" s="24" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1084,7 +1253,7 @@
       <c r="J12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K12" s="24" t="s">
+      <c r="K12" s="23" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1113,7 +1282,7 @@
       <c r="J13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K13" s="24" t="s">
+      <c r="K13" s="23" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1142,7 +1311,7 @@
       <c r="J14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K14" s="24" t="s">
+      <c r="K14" s="23" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1171,7 +1340,7 @@
       <c r="J15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K15" s="24" t="s">
+      <c r="K15" s="23" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1200,7 +1369,7 @@
       <c r="J16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K16" s="24" t="s">
+      <c r="K16" s="23" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1229,7 +1398,7 @@
       <c r="J17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K17" s="24" t="s">
+      <c r="K17" s="23" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1258,7 +1427,7 @@
       <c r="J18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K18" s="24" t="s">
+      <c r="K18" s="23" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1287,7 +1456,7 @@
       <c r="J19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K19" s="24" t="s">
+      <c r="K19" s="23" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1316,7 +1485,7 @@
       <c r="J20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K20" s="24" t="s">
+      <c r="K20" s="23" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1345,7 +1514,7 @@
       <c r="J21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K21" s="24" t="s">
+      <c r="K21" s="23" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1374,7 +1543,7 @@
       <c r="J22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K22" s="24" t="s">
+      <c r="K22" s="23" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1403,7 +1572,7 @@
       <c r="J23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K23" s="24" t="s">
+      <c r="K23" s="23" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1432,7 +1601,7 @@
       <c r="J24" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K24" s="24" t="s">
+      <c r="K24" s="23" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1461,7 +1630,7 @@
       <c r="J25" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K25" s="24" t="s">
+      <c r="K25" s="23" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1490,7 +1659,7 @@
       <c r="J26" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K26" s="24" t="s">
+      <c r="K26" s="23" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1519,7 +1688,7 @@
       <c r="J27" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K27" s="24" t="s">
+      <c r="K27" s="23" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1548,7 +1717,7 @@
       <c r="J28" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K28" s="24" t="s">
+      <c r="K28" s="23" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1577,7 +1746,7 @@
       <c r="J29" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K29" s="24" t="s">
+      <c r="K29" s="23" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1606,7 +1775,7 @@
       <c r="J30" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K30" s="24" t="s">
+      <c r="K30" s="23" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1635,7 +1804,7 @@
       <c r="J31" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K31" s="24" t="s">
+      <c r="K31" s="23" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1664,7 +1833,7 @@
       <c r="J32" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K32" s="24" t="s">
+      <c r="K32" s="23" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1693,7 +1862,7 @@
       <c r="J33" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K33" s="24" t="s">
+      <c r="K33" s="23" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1723,7 +1892,7 @@
       <c r="J34" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="K34" s="25" t="s">
+      <c r="K34" s="24" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1753,7 +1922,7 @@
       <c r="J35" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="K35" s="25" t="s">
+      <c r="K35" s="24" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1782,7 +1951,7 @@
       <c r="J36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K36" s="24" t="s">
+      <c r="K36" s="23" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1811,7 +1980,7 @@
       <c r="J37" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K37" s="24" t="s">
+      <c r="K37" s="23" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1840,7 +2009,7 @@
       <c r="J38" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K38" s="24" t="s">
+      <c r="K38" s="23" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1866,7 +2035,7 @@
       <c r="G39" s="7">
         <v>29</v>
       </c>
-      <c r="J39" s="24" t="s">
+      <c r="J39" s="23" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1895,7 +2064,7 @@
       <c r="J40" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K40" s="24" t="s">
+      <c r="K40" s="23" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1924,7 +2093,7 @@
       <c r="J41" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K41" s="24" t="s">
+      <c r="K41" s="23" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1953,7 +2122,7 @@
       <c r="J42" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K42" s="24" t="s">
+      <c r="K42" s="23" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1969,24 +2138,1562 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="33.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="65.140625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="3.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.140625" style="7" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="7" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="34.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="34.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="31.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="31.28515625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="30"/>
+      <c r="F1" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="L2" s="34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="15">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="15">
+        <v>2</v>
+      </c>
+      <c r="D4" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="44">
+        <v>3</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="42">
+        <v>0</v>
+      </c>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="J5" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="L5" s="41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="15">
+        <v>4</v>
+      </c>
+      <c r="D6" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="44">
+        <v>6</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="42">
+        <v>1</v>
+      </c>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="J7" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="L7" s="41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="15">
+        <v>7</v>
+      </c>
+      <c r="D8" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1</v>
+      </c>
+      <c r="I8" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="15">
+        <v>40</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="7">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J9" s="50" t="s">
+        <v>110</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="15">
+        <v>15</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="7">
+        <v>2</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L10" s="47" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="15">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L11" s="48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" s="16">
+        <v>16</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="7">
+        <v>2</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L12" s="48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="16">
+        <v>13</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="7">
+        <v>3</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L13" s="48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="16">
+        <v>14</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="7">
+        <v>4</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L14" s="48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="18">
+        <v>30</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="20">
+        <v>7</v>
+      </c>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L15" s="48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="16">
+        <v>31</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="7">
+        <v>8</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L16" s="48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="16">
+        <v>39</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="7">
+        <v>4</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L17" s="47" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="16">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="7">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L18" s="48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="16">
+        <v>19</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="7">
+        <v>2</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L19" s="48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="16">
+        <v>23</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="7">
+        <v>3</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L20" s="48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="16">
+        <v>22</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="7">
+        <v>4</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L21" s="48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="16">
+        <v>12</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L22" s="48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="16">
+        <v>27</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="7">
+        <v>6</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L23" s="48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" s="16">
+        <v>18</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="7">
+        <v>7</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L24" s="48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" s="16">
+        <v>26</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="7">
+        <v>5</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L25" s="47" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" s="16">
+        <v>11</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" s="7">
+        <v>5</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L26" s="48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" s="16">
+        <v>29</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" s="7">
+        <v>2</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L27" s="48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="16">
+        <v>25</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F28" s="7">
+        <v>3</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L28" s="48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="16">
+        <v>32</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" s="7">
+        <v>4</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L29" s="48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" s="16">
+        <v>20</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" s="7">
+        <v>5</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L30" s="48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" s="16">
+        <v>33</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F31" s="7">
+        <v>6</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L31" s="47" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="16">
+        <v>35</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F32" s="7">
+        <v>1</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L32" s="48" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="16">
+        <v>24</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F33" s="7">
+        <v>2</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L33" s="48" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="16">
+        <v>17</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F34" s="7">
+        <v>7</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L34" s="47" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35" s="16">
+        <v>38</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F35" s="7">
+        <v>1</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L35" s="48" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" s="16">
+        <v>36</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F36" s="7">
+        <v>1</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L36" s="49" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" s="16">
+        <v>37</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37" s="7">
+        <v>5</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L37" s="49" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" s="18">
+        <v>41</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F38" s="20">
+        <v>6</v>
+      </c>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J38" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L38" s="49" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" s="18">
+        <v>9</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F39" s="20">
+        <v>9</v>
+      </c>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J39" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L39" s="47" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" s="16">
+        <v>21</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F40" s="7">
+        <v>1</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L40" s="48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" s="16">
+        <v>10</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F41" s="7">
+        <v>2</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L41" s="48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42" s="16">
+        <v>34</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F42" s="7">
+        <v>3</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L42" s="48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="C43" s="40">
+        <v>5</v>
+      </c>
+      <c r="D43" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="E43" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="F43" s="42">
+        <v>2</v>
+      </c>
+      <c r="G43" s="42"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="J43" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="K43" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="L43" s="41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C44" s="16">
+        <v>42</v>
+      </c>
+      <c r="D44" s="57" t="s">
+        <v>112</v>
+      </c>
+      <c r="F44" s="7">
+        <v>2</v>
+      </c>
+      <c r="I44" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45" s="16">
+        <v>44</v>
+      </c>
+      <c r="D45" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F45" s="7">
+        <v>2</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J45" s="58" t="s">
+        <v>112</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" s="15">
+        <v>45</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F46" s="7">
+        <v>1</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L46" s="56" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47" s="15">
+        <v>46</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F47" s="7">
+        <v>2</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L47" s="56" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C48" s="15">
+        <v>43</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F48" s="7">
+        <v>3</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L48" s="56" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:L1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>